<commit_message>
changed files in Data
</commit_message>
<xml_diff>
--- a/PM/Data/Building Data and Energy Validation.xlsx
+++ b/PM/Data/Building Data and Energy Validation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iA\Desktop\PM\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prakh\Documents\Thesis\PM\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33537E8B-3E6F-4257-89C1-3216C9BA6BCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6443156-1CEB-4D56-869F-1E65FFF10132}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13470" windowHeight="10290" xr2:uid="{3C5C305A-6140-4C8D-952A-58D32A290B96}"/>
   </bookViews>
@@ -19,10 +19,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Building Stock Data'!$A$1:$F$1936</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -11850,7 +11855,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12113,7 +12118,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="656181304"/>
@@ -12175,7 +12180,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="656182944"/>
@@ -12223,7 +12228,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -12306,7 +12311,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -12569,7 +12574,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="465114976"/>
@@ -12631,7 +12636,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="465113664"/>
@@ -12679,7 +12684,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -14178,8 +14183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F7F7D89-9086-431F-8D6D-8545BF490508}">
   <dimension ref="A1:V1938"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="F19" workbookViewId="0">
+      <selection activeCell="AB44" sqref="AB44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14225,7 +14230,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="str">
-        <f>VLOOKUP(A3,Q3:V1938,6)</f>
+        <f t="shared" ref="B3:B34" si="0">VLOOKUP(A3,Q3:V1938,6)</f>
         <v>Residential</v>
       </c>
       <c r="C3">
@@ -14276,7 +14281,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="str">
-        <f>VLOOKUP(A4,Q4:V1939,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C4">
@@ -14286,7 +14291,7 @@
         <v>6508.3729999999996</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E51" si="0">C4*1000/D4</f>
+        <f t="shared" ref="E4:E51" si="1">C4*1000/D4</f>
         <v>25.356260312677225</v>
       </c>
       <c r="F4">
@@ -14300,7 +14305,7 @@
         <v>1040.1420000000001</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I51" si="1">H4/D4*1000</f>
+        <f t="shared" ref="I4:I51" si="2">H4/D4*1000</f>
         <v>159.81597858635331</v>
       </c>
       <c r="Q4" t="s">
@@ -14327,7 +14332,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="str">
-        <f>VLOOKUP(A5,Q5:V1940,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C5">
@@ -14337,7 +14342,7 @@
         <v>1463.1030000000001</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>72.435775198328486</v>
       </c>
       <c r="F5">
@@ -14347,11 +14352,11 @@
         <v>311.79599999999999</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H4:H51" si="2">C5+F5+G5</f>
+        <f t="shared" ref="H5:H51" si="3">C5+F5+G5</f>
         <v>457.94399999999996</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>312.99505229638646</v>
       </c>
       <c r="Q5" t="s">
@@ -14378,7 +14383,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="str">
-        <f>VLOOKUP(A6,Q6:V1941,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C6">
@@ -14388,7 +14393,7 @@
         <v>724.34500000000003</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.7859031262727</v>
       </c>
       <c r="F6">
@@ -14429,7 +14434,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="str">
-        <f>VLOOKUP(A7,Q7:V1942,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C7">
@@ -14439,7 +14444,7 @@
         <v>736.70399999999995</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.800386586743123</v>
       </c>
       <c r="F7">
@@ -14449,11 +14454,11 @@
         <v>101.006</v>
       </c>
       <c r="H7">
+        <f t="shared" si="3"/>
+        <v>148.00800000000001</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="2"/>
-        <v>148.00800000000001</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="1"/>
         <v>200.90565545999482</v>
       </c>
       <c r="Q7" t="s">
@@ -14480,7 +14485,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="str">
-        <f>VLOOKUP(A8,Q8:V1943,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C8">
@@ -14490,7 +14495,7 @@
         <v>4859.24</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.779109490372981</v>
       </c>
       <c r="F8">
@@ -14500,11 +14505,11 @@
         <v>731.64499999999998</v>
       </c>
       <c r="H8">
+        <f t="shared" si="3"/>
+        <v>1041.5630000000001</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="2"/>
-        <v>1041.5630000000001</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="1"/>
         <v>214.3468937529326</v>
       </c>
       <c r="Q8" t="s">
@@ -14531,7 +14536,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="str">
-        <f>VLOOKUP(A9,Q9:V1944,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C9">
@@ -14541,7 +14546,7 @@
         <v>1683.2380000000001</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.46376329431726</v>
       </c>
       <c r="F9">
@@ -14551,11 +14556,11 @@
         <v>162.39599999999999</v>
       </c>
       <c r="H9">
+        <f t="shared" si="3"/>
+        <v>250.70499999999998</v>
+      </c>
+      <c r="I9">
         <f t="shared" si="2"/>
-        <v>250.70499999999998</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="1"/>
         <v>148.94209850300433</v>
       </c>
       <c r="Q9" t="s">
@@ -14582,7 +14587,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="str">
-        <f>VLOOKUP(A10,Q10:V1945,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C10">
@@ -14592,7 +14597,7 @@
         <v>734.65599999999995</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.786316316752334</v>
       </c>
       <c r="F10">
@@ -14602,11 +14607,11 @@
         <v>97.17</v>
       </c>
       <c r="H10">
+        <f t="shared" si="3"/>
+        <v>144.03100000000001</v>
+      </c>
+      <c r="I10">
         <f t="shared" si="2"/>
-        <v>144.03100000000001</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
         <v>196.05230202979357</v>
       </c>
       <c r="Q10" t="s">
@@ -14633,7 +14638,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="str">
-        <f>VLOOKUP(A11,Q11:V1946,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C11">
@@ -14643,7 +14648,7 @@
         <v>764.70399999999995</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.815541699794956</v>
       </c>
       <c r="F11">
@@ -14653,11 +14658,11 @@
         <v>162.071</v>
       </c>
       <c r="H11">
+        <f t="shared" si="3"/>
+        <v>210.87099999999998</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="2"/>
-        <v>210.87099999999998</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
         <v>275.75506339707914</v>
       </c>
       <c r="Q11" t="s">
@@ -14684,7 +14689,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="str">
-        <f>VLOOKUP(A12,Q12:V1947,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C12">
@@ -14694,7 +14699,7 @@
         <v>4902.759</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.765116743449965</v>
       </c>
       <c r="F12">
@@ -14704,11 +14709,11 @@
         <v>793.26099999999997</v>
       </c>
       <c r="H12">
+        <f t="shared" si="3"/>
+        <v>1105.886</v>
+      </c>
+      <c r="I12">
         <f t="shared" si="2"/>
-        <v>1105.886</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
         <v>225.56401405820679</v>
       </c>
       <c r="Q12" t="s">
@@ -14735,7 +14740,7 @@
         <v>17</v>
       </c>
       <c r="B13" t="str">
-        <f>VLOOKUP(A13,Q13:V1948,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C13">
@@ -14745,7 +14750,7 @@
         <v>3835.8760000000002</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.78021604452281</v>
       </c>
       <c r="F13">
@@ -14755,11 +14760,11 @@
         <v>572.98400000000004</v>
       </c>
       <c r="H13">
+        <f t="shared" si="3"/>
+        <v>817.63700000000006</v>
+      </c>
+      <c r="I13">
         <f t="shared" si="2"/>
-        <v>817.63700000000006</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
         <v>213.15522191019733</v>
       </c>
       <c r="Q13" t="s">
@@ -14786,7 +14791,7 @@
         <v>18</v>
       </c>
       <c r="B14" t="str">
-        <f>VLOOKUP(A14,Q14:V1949,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C14">
@@ -14796,7 +14801,7 @@
         <v>294.71600000000001</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.709496600116722</v>
       </c>
       <c r="F14">
@@ -14806,11 +14811,11 @@
         <v>34.069000000000003</v>
       </c>
       <c r="H14">
+        <f t="shared" si="3"/>
+        <v>42.241</v>
+      </c>
+      <c r="I14">
         <f t="shared" si="2"/>
-        <v>42.241</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
         <v>143.32781389541117</v>
       </c>
       <c r="Q14" t="s">
@@ -14837,7 +14842,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="str">
-        <f>VLOOKUP(A15,Q15:V1950,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C15">
@@ -14847,7 +14852,7 @@
         <v>3195.5360000000001</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.75956959959143</v>
       </c>
       <c r="F15">
@@ -14857,11 +14862,11 @@
         <v>302.02999999999997</v>
       </c>
       <c r="H15">
+        <f t="shared" si="3"/>
+        <v>505.77599999999995</v>
+      </c>
+      <c r="I15">
         <f t="shared" si="2"/>
-        <v>505.77599999999995</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
         <v>158.27579473365344</v>
       </c>
       <c r="Q15" t="s">
@@ -14888,7 +14893,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="str">
-        <f>VLOOKUP(A16,Q16:V1951,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C16">
@@ -14908,11 +14913,11 @@
         <v>40.771999999999998</v>
       </c>
       <c r="H16">
+        <f t="shared" si="3"/>
+        <v>53.150999999999996</v>
+      </c>
+      <c r="I16">
         <f t="shared" si="2"/>
-        <v>53.150999999999996</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
         <v>753.10303785989572</v>
       </c>
       <c r="Q16" t="s">
@@ -14939,7 +14944,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="str">
-        <f>VLOOKUP(A17,Q17:V1952,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C17">
@@ -14949,7 +14954,7 @@
         <v>1588.8309999999999</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.768267361349324</v>
       </c>
       <c r="F17">
@@ -14959,11 +14964,11 @@
         <v>163.119</v>
       </c>
       <c r="H17">
+        <f t="shared" si="3"/>
+        <v>264.43599999999998</v>
+      </c>
+      <c r="I17">
         <f t="shared" si="2"/>
-        <v>264.43599999999998</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
         <v>166.43431554394394</v>
       </c>
       <c r="Q17" t="s">
@@ -14990,7 +14995,7 @@
         <v>23</v>
       </c>
       <c r="B18" t="str">
-        <f>VLOOKUP(A18,Q18:V1953,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C18">
@@ -15000,7 +15005,7 @@
         <v>3150.67</v>
       </c>
       <c r="E18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.955285701136582</v>
       </c>
       <c r="F18">
@@ -15010,11 +15015,11 @@
         <v>341.19400000000002</v>
       </c>
       <c r="H18">
+        <f t="shared" si="3"/>
+        <v>542.69600000000003</v>
+      </c>
+      <c r="I18">
         <f t="shared" si="2"/>
-        <v>542.69600000000003</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
         <v>172.2478076091752</v>
       </c>
       <c r="Q18" t="s">
@@ -15041,7 +15046,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="str">
-        <f>VLOOKUP(A19,Q19:V1954,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C19">
@@ -15051,7 +15056,7 @@
         <v>1226.625</v>
       </c>
       <c r="E19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.773361866911237</v>
       </c>
       <c r="F19">
@@ -15061,11 +15066,11 @@
         <v>132.34800000000001</v>
       </c>
       <c r="H19">
+        <f t="shared" si="3"/>
+        <v>210.57400000000001</v>
+      </c>
+      <c r="I19">
         <f t="shared" si="2"/>
-        <v>210.57400000000001</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
         <v>171.66941811882197</v>
       </c>
       <c r="Q19" t="s">
@@ -15092,7 +15097,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="str">
-        <f>VLOOKUP(A20,Q20:V1955,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C20">
@@ -15102,7 +15107,7 @@
         <v>271.005</v>
       </c>
       <c r="E20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.847530488367376</v>
       </c>
       <c r="F20">
@@ -15112,11 +15117,11 @@
         <v>82.028999999999996</v>
       </c>
       <c r="H20">
+        <f t="shared" si="3"/>
+        <v>99.331999999999994</v>
+      </c>
+      <c r="I20">
         <f t="shared" si="2"/>
-        <v>99.331999999999994</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
         <v>366.53198280474533</v>
       </c>
       <c r="Q20" t="s">
@@ -15143,7 +15148,7 @@
         <v>26</v>
       </c>
       <c r="B21" t="str">
-        <f>VLOOKUP(A21,Q21:V1956,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C21">
@@ -15153,7 +15158,7 @@
         <v>1378.222</v>
       </c>
       <c r="E21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.768391449273047</v>
       </c>
       <c r="F21">
@@ -15163,11 +15168,11 @@
         <v>142.05500000000001</v>
       </c>
       <c r="H21">
+        <f t="shared" si="3"/>
+        <v>229.94200000000001</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="2"/>
-        <v>229.94200000000001</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
         <v>166.83959478226296</v>
       </c>
       <c r="Q21" t="s">
@@ -15194,7 +15199,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="str">
-        <f>VLOOKUP(A22,Q22:V1957,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C22">
@@ -15204,7 +15209,7 @@
         <v>936.36800000000005</v>
       </c>
       <c r="E22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.794362900056385</v>
       </c>
       <c r="F22">
@@ -15214,11 +15219,11 @@
         <v>193.095</v>
       </c>
       <c r="H22">
+        <f t="shared" si="3"/>
+        <v>252.82999999999998</v>
+      </c>
+      <c r="I22">
         <f t="shared" si="2"/>
-        <v>252.82999999999998</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
         <v>270.01136305384205</v>
       </c>
       <c r="Q22" t="s">
@@ -15245,7 +15250,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="str">
-        <f>VLOOKUP(A23,Q23:V1958,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C23">
@@ -15255,7 +15260,7 @@
         <v>1132.027</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.773213889774709</v>
       </c>
       <c r="F23">
@@ -15265,11 +15270,11 @@
         <v>121.916</v>
       </c>
       <c r="H23">
+        <f t="shared" si="3"/>
+        <v>194.10899999999998</v>
+      </c>
+      <c r="I23">
         <f t="shared" si="2"/>
-        <v>194.10899999999998</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
         <v>171.47029178632664</v>
       </c>
       <c r="Q23" t="s">
@@ -15296,7 +15301,7 @@
         <v>29</v>
       </c>
       <c r="B24" t="str">
-        <f>VLOOKUP(A24,Q24:V1959,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C24">
@@ -15306,7 +15311,7 @@
         <v>933.58299999999997</v>
       </c>
       <c r="E24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.792935389783239</v>
       </c>
       <c r="F24">
@@ -15316,11 +15321,11 @@
         <v>186.727</v>
       </c>
       <c r="H24">
+        <f t="shared" si="3"/>
+        <v>246.28300000000002</v>
+      </c>
+      <c r="I24">
         <f t="shared" si="2"/>
-        <v>246.28300000000002</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
         <v>263.80407526700895</v>
       </c>
       <c r="Q24" t="s">
@@ -15347,7 +15352,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="str">
-        <f>VLOOKUP(A25,Q25:V1960,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C25">
@@ -15357,7 +15362,7 @@
         <v>615.39700000000005</v>
       </c>
       <c r="E25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.786466297365763</v>
       </c>
       <c r="F25">
@@ -15367,11 +15372,11 @@
         <v>77.643000000000001</v>
       </c>
       <c r="H25">
+        <f t="shared" si="3"/>
+        <v>116.89699999999999</v>
+      </c>
+      <c r="I25">
         <f t="shared" si="2"/>
-        <v>116.89699999999999</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="1"/>
         <v>189.9538021797311</v>
       </c>
       <c r="Q25" t="s">
@@ -15398,7 +15403,7 @@
         <v>31</v>
       </c>
       <c r="B26" t="str">
-        <f>VLOOKUP(A26,Q26:V1961,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C26">
@@ -15408,7 +15413,7 @@
         <v>1230.9929999999999</v>
       </c>
       <c r="E26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.783465868611763</v>
       </c>
       <c r="F26">
@@ -15418,11 +15423,11 @@
         <v>107.61199999999999</v>
       </c>
       <c r="H26">
+        <f t="shared" si="3"/>
+        <v>186.12899999999999</v>
+      </c>
+      <c r="I26">
         <f t="shared" si="2"/>
-        <v>186.12899999999999</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="1"/>
         <v>151.20232202782631</v>
       </c>
       <c r="Q26" t="s">
@@ -15449,7 +15454,7 @@
         <v>33</v>
       </c>
       <c r="B27" t="str">
-        <f>VLOOKUP(A27,Q27:V1962,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C27">
@@ -15459,7 +15464,7 @@
         <v>2404.6849999999999</v>
       </c>
       <c r="E27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.761365833778648</v>
       </c>
       <c r="F27">
@@ -15469,11 +15474,11 @@
         <v>223.71</v>
       </c>
       <c r="H27">
+        <f t="shared" si="3"/>
+        <v>377.036</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="2"/>
-        <v>377.036</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="1"/>
         <v>156.79226177233193</v>
       </c>
       <c r="Q27" t="s">
@@ -15500,7 +15505,7 @@
         <v>34</v>
       </c>
       <c r="B28" t="str">
-        <f>VLOOKUP(A28,Q28:V1963,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C28">
@@ -15510,7 +15515,7 @@
         <v>422.209</v>
       </c>
       <c r="E28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.826209294448958</v>
       </c>
       <c r="F28">
@@ -15520,11 +15525,11 @@
         <v>108.45399999999999</v>
       </c>
       <c r="H28">
+        <f t="shared" si="3"/>
+        <v>135.40199999999999</v>
+      </c>
+      <c r="I28">
         <f t="shared" si="2"/>
-        <v>135.40199999999999</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="1"/>
         <v>320.69899031048601</v>
       </c>
       <c r="Q28" t="s">
@@ -15551,7 +15556,7 @@
         <v>36</v>
       </c>
       <c r="B29" t="str">
-        <f>VLOOKUP(A29,Q29:V1964,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C29">
@@ -15561,7 +15566,7 @@
         <v>3504.1660000000002</v>
       </c>
       <c r="E29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>84.076211001419452</v>
       </c>
       <c r="F29">
@@ -15571,11 +15576,11 @@
         <v>550.71100000000001</v>
       </c>
       <c r="H29">
+        <f t="shared" si="3"/>
+        <v>845.32799999999997</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="2"/>
-        <v>845.32799999999997</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="1"/>
         <v>241.23514696506956</v>
       </c>
       <c r="Q29" t="s">
@@ -15602,7 +15607,7 @@
         <v>37</v>
       </c>
       <c r="B30" t="str">
-        <f>VLOOKUP(A30,Q30:V1965,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C30">
@@ -15612,7 +15617,7 @@
         <v>824.75599999999997</v>
       </c>
       <c r="E30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.790987880051802</v>
       </c>
       <c r="F30">
@@ -15622,11 +15627,11 @@
         <v>106.982</v>
       </c>
       <c r="H30">
+        <f t="shared" si="3"/>
+        <v>159.59399999999999</v>
+      </c>
+      <c r="I30">
         <f t="shared" si="2"/>
-        <v>159.59399999999999</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="1"/>
         <v>193.50450315002254</v>
       </c>
       <c r="Q30" t="s">
@@ -15653,7 +15658,7 @@
         <v>38</v>
       </c>
       <c r="B31" t="str">
-        <f>VLOOKUP(A31,Q31:V1966,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C31">
@@ -15663,7 +15668,7 @@
         <v>461.68599999999998</v>
       </c>
       <c r="E31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.822598042825646</v>
       </c>
       <c r="F31">
@@ -15673,11 +15678,11 @@
         <v>113.97499999999999</v>
       </c>
       <c r="H31">
+        <f t="shared" si="3"/>
+        <v>143.441</v>
+      </c>
+      <c r="I31">
         <f t="shared" si="2"/>
-        <v>143.441</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="1"/>
         <v>310.68951625130501</v>
       </c>
       <c r="Q31" t="s">
@@ -15704,7 +15709,7 @@
         <v>40</v>
       </c>
       <c r="B32" t="str">
-        <f>VLOOKUP(A32,Q32:V1967,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C32">
@@ -15714,7 +15719,7 @@
         <v>7057.0569999999998</v>
       </c>
       <c r="E32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.769642217712004</v>
       </c>
       <c r="F32">
@@ -15724,11 +15729,11 @@
         <v>595.28300000000002</v>
       </c>
       <c r="H32">
+        <f t="shared" si="3"/>
+        <v>1045.309</v>
+      </c>
+      <c r="I32">
         <f t="shared" si="2"/>
-        <v>1045.309</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
         <v>148.12251055928837</v>
       </c>
       <c r="Q32" t="s">
@@ -15755,7 +15760,7 @@
         <v>44</v>
       </c>
       <c r="B33" t="str">
-        <f>VLOOKUP(A33,Q33:V1968,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C33">
@@ -15765,7 +15770,7 @@
         <v>459.74799999999999</v>
       </c>
       <c r="E33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>95.704603391423134</v>
       </c>
       <c r="F33">
@@ -15775,11 +15780,11 @@
         <v>229.65899999999999</v>
       </c>
       <c r="H33">
+        <f t="shared" si="3"/>
+        <v>273.65899999999999</v>
+      </c>
+      <c r="I33">
         <f t="shared" si="2"/>
-        <v>273.65899999999999</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="1"/>
         <v>595.23695589757858</v>
       </c>
       <c r="Q33" t="s">
@@ -15806,7 +15811,7 @@
         <v>45</v>
       </c>
       <c r="B34" t="str">
-        <f>VLOOKUP(A34,Q34:V1969,6)</f>
+        <f t="shared" si="0"/>
         <v>Residential</v>
       </c>
       <c r="C34">
@@ -15816,7 +15821,7 @@
         <v>2048.1529999999998</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.765744063065604</v>
       </c>
       <c r="F34">
@@ -15826,11 +15831,11 @@
         <v>188.31</v>
       </c>
       <c r="H34">
+        <f t="shared" si="3"/>
+        <v>318.91200000000003</v>
+      </c>
+      <c r="I34">
         <f t="shared" si="2"/>
-        <v>318.91200000000003</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="1"/>
         <v>155.70711758350086</v>
       </c>
       <c r="Q34" t="s">
@@ -15857,7 +15862,7 @@
         <v>46</v>
       </c>
       <c r="B35" t="str">
-        <f>VLOOKUP(A35,Q35:V1970,6)</f>
+        <f t="shared" ref="B35:B66" si="4">VLOOKUP(A35,Q35:V1970,6)</f>
         <v>Residential</v>
       </c>
       <c r="C35">
@@ -15867,7 +15872,7 @@
         <v>13537.464</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>66.667139428773368</v>
       </c>
       <c r="F35">
@@ -15877,11 +15882,11 @@
         <v>1071.6379999999999</v>
       </c>
       <c r="H35">
+        <f t="shared" si="3"/>
+        <v>1974.1419999999998</v>
+      </c>
+      <c r="I35">
         <f t="shared" si="2"/>
-        <v>1974.1419999999998</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="1"/>
         <v>145.82805169417253</v>
       </c>
       <c r="Q35" t="s">
@@ -15908,7 +15913,7 @@
         <v>47</v>
       </c>
       <c r="B36" t="str">
-        <f>VLOOKUP(A36,Q36:V1971,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C36">
@@ -15918,7 +15923,7 @@
         <v>474.86700000000002</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.830504120100997</v>
       </c>
       <c r="F36">
@@ -15928,11 +15933,11 @@
         <v>115.214</v>
       </c>
       <c r="H36">
+        <f t="shared" si="3"/>
+        <v>145.52500000000001</v>
+      </c>
+      <c r="I36">
         <f t="shared" si="2"/>
-        <v>145.52500000000001</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="1"/>
         <v>306.4542282365378</v>
       </c>
       <c r="Q36" t="s">
@@ -15959,7 +15964,7 @@
         <v>50</v>
       </c>
       <c r="B37" t="str">
-        <f>VLOOKUP(A37,Q37:V1972,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C37">
@@ -15969,7 +15974,7 @@
         <v>629.10500000000002</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>121.89062239212849</v>
       </c>
       <c r="F37">
@@ -15979,11 +15984,11 @@
         <v>182.958</v>
       </c>
       <c r="H37">
+        <f t="shared" si="3"/>
+        <v>289.39300000000003</v>
+      </c>
+      <c r="I37">
         <f t="shared" si="2"/>
-        <v>289.39300000000003</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="1"/>
         <v>460.00747093092571</v>
       </c>
       <c r="Q37" t="s">
@@ -16010,7 +16015,7 @@
         <v>51</v>
       </c>
       <c r="B38" t="str">
-        <f>VLOOKUP(A38,Q38:V1973,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C38">
@@ -16020,7 +16025,7 @@
         <v>65.626000000000005</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>135.89126260933165</v>
       </c>
       <c r="F38">
@@ -16030,11 +16035,11 @@
         <v>38.015999999999998</v>
       </c>
       <c r="H38">
+        <f t="shared" si="3"/>
+        <v>49.113999999999997</v>
+      </c>
+      <c r="I38">
         <f t="shared" si="2"/>
-        <v>49.113999999999997</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="1"/>
         <v>748.39240544905977</v>
       </c>
       <c r="Q38" t="s">
@@ -16061,7 +16066,7 @@
         <v>9</v>
       </c>
       <c r="B39" t="str">
-        <f>VLOOKUP(A39,Q39:V1974,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C39">
@@ -16071,7 +16076,7 @@
         <v>5711.4650000000001</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27.225414145057353</v>
       </c>
       <c r="F39">
@@ -16081,11 +16086,11 @@
         <v>264.66000000000003</v>
       </c>
       <c r="H39">
+        <f t="shared" si="3"/>
+        <v>437.43700000000001</v>
+      </c>
+      <c r="I39">
         <f t="shared" si="2"/>
-        <v>437.43700000000001</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="1"/>
         <v>76.589281384023181</v>
       </c>
       <c r="Q39" t="s">
@@ -16112,7 +16117,7 @@
         <v>10</v>
       </c>
       <c r="B40" t="str">
-        <f>VLOOKUP(A40,Q40:V1975,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C40">
@@ -16122,7 +16127,7 @@
         <v>5822.2120000000004</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27.89730088839087</v>
       </c>
       <c r="F40">
@@ -16132,11 +16137,11 @@
         <v>235.95500000000001</v>
       </c>
       <c r="H40">
+        <f t="shared" si="3"/>
+        <v>442.36400000000003</v>
+      </c>
+      <c r="I40">
         <f t="shared" si="2"/>
-        <v>442.36400000000003</v>
-      </c>
-      <c r="I40">
-        <f t="shared" si="1"/>
         <v>75.978683016008347</v>
       </c>
       <c r="Q40" t="s">
@@ -16163,7 +16168,7 @@
         <v>11</v>
       </c>
       <c r="B41" t="str">
-        <f>VLOOKUP(A41,Q41:V1976,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C41">
@@ -16173,7 +16178,7 @@
         <v>1869.394</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.781096975811415</v>
       </c>
       <c r="F41">
@@ -16183,11 +16188,11 @@
         <v>99.147999999999996</v>
       </c>
       <c r="H41">
+        <f t="shared" si="3"/>
+        <v>218.38</v>
+      </c>
+      <c r="I41">
         <f t="shared" si="2"/>
-        <v>218.38</v>
-      </c>
-      <c r="I41">
-        <f t="shared" si="1"/>
         <v>116.81860538762828</v>
       </c>
       <c r="Q41" t="s">
@@ -16214,7 +16219,7 @@
         <v>32</v>
       </c>
       <c r="B42" t="str">
-        <f>VLOOKUP(A42,Q42:V1977,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C42">
@@ -16224,7 +16229,7 @@
         <v>1513.183</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.771533251430924</v>
       </c>
       <c r="F42">
@@ -16234,11 +16239,11 @@
         <v>88.155000000000001</v>
       </c>
       <c r="H42">
+        <f t="shared" si="3"/>
+        <v>184.65300000000002</v>
+      </c>
+      <c r="I42">
         <f t="shared" si="2"/>
-        <v>184.65300000000002</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="1"/>
         <v>122.02952319712819</v>
       </c>
       <c r="Q42" t="s">
@@ -16265,7 +16270,7 @@
         <v>39</v>
       </c>
       <c r="B43" t="str">
-        <f>VLOOKUP(A43,Q43:V1978,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C43">
@@ -16275,7 +16280,7 @@
         <v>8024.4219999999996</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29.524369481066675</v>
       </c>
       <c r="F43">
@@ -16285,11 +16290,11 @@
         <v>580.97799999999995</v>
       </c>
       <c r="H43">
+        <f t="shared" si="3"/>
+        <v>884.96299999999997</v>
+      </c>
+      <c r="I43">
         <f t="shared" si="2"/>
-        <v>884.96299999999997</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="1"/>
         <v>110.28370641524089</v>
       </c>
       <c r="Q43" t="s">
@@ -16316,7 +16321,7 @@
         <v>41</v>
       </c>
       <c r="B44" t="str">
-        <f>VLOOKUP(A44,Q44:V1979,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C44">
@@ -16326,7 +16331,7 @@
         <v>4340.152</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.778411447341014</v>
       </c>
       <c r="F44">
@@ -16336,11 +16341,11 @@
         <v>231.852</v>
       </c>
       <c r="H44">
+        <f t="shared" si="3"/>
+        <v>508.65999999999997</v>
+      </c>
+      <c r="I44">
         <f t="shared" si="2"/>
-        <v>508.65999999999997</v>
-      </c>
-      <c r="I44">
-        <f t="shared" si="1"/>
         <v>117.19866032341723</v>
       </c>
       <c r="Q44" t="s">
@@ -16367,7 +16372,7 @@
         <v>42</v>
       </c>
       <c r="B45" t="str">
-        <f>VLOOKUP(A45,Q45:V1980,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C45">
@@ -16377,7 +16382,7 @@
         <v>954.19899999999996</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.774956796223854</v>
       </c>
       <c r="F45">
@@ -16387,11 +16392,11 @@
         <v>55.411000000000001</v>
       </c>
       <c r="H45">
+        <f t="shared" si="3"/>
+        <v>116.265</v>
+      </c>
+      <c r="I45">
         <f t="shared" si="2"/>
-        <v>116.265</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="1"/>
         <v>121.8456527411997</v>
       </c>
       <c r="Q45" t="s">
@@ -16418,7 +16423,7 @@
         <v>43</v>
       </c>
       <c r="B46" t="str">
-        <f>VLOOKUP(A46,Q46:V1981,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C46">
@@ -16428,7 +16433,7 @@
         <v>5778.7860000000001</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.785888593209712</v>
       </c>
       <c r="F46">
@@ -16438,11 +16443,11 @@
         <v>240.89099999999999</v>
       </c>
       <c r="H46">
+        <f t="shared" si="3"/>
+        <v>609.49599999999998</v>
+      </c>
+      <c r="I46">
         <f t="shared" si="2"/>
-        <v>609.49599999999998</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="1"/>
         <v>105.47128756801169</v>
       </c>
       <c r="Q46" t="s">
@@ -16469,7 +16474,7 @@
         <v>21</v>
       </c>
       <c r="B47" t="str">
-        <f>VLOOKUP(A47,Q47:V1982,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C47">
@@ -16479,7 +16484,7 @@
         <v>1076.114</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.763690464021465</v>
       </c>
       <c r="F47">
@@ -16489,11 +16494,11 @@
         <v>75.515000000000001</v>
       </c>
       <c r="H47">
+        <f t="shared" si="3"/>
+        <v>144.13200000000001</v>
+      </c>
+      <c r="I47">
         <f t="shared" si="2"/>
-        <v>144.13200000000001</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="1"/>
         <v>133.93748246003676</v>
       </c>
       <c r="Q47" t="s">
@@ -16520,7 +16525,7 @@
         <v>35</v>
       </c>
       <c r="B48" t="str">
-        <f>VLOOKUP(A48,Q48:V1983,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C48">
@@ -16530,7 +16535,7 @@
         <v>1449.5840000000001</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>63.762431152661726</v>
       </c>
       <c r="F48">
@@ -16540,11 +16545,11 @@
         <v>101.43600000000001</v>
       </c>
       <c r="H48">
+        <f t="shared" si="3"/>
+        <v>193.86500000000001</v>
+      </c>
+      <c r="I48">
         <f t="shared" si="2"/>
-        <v>193.86500000000001</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="1"/>
         <v>133.73836907692137</v>
       </c>
       <c r="Q48" t="s">
@@ -16571,7 +16576,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="str">
-        <f>VLOOKUP(A49,Q49:V1984,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C49">
@@ -16581,18 +16586,18 @@
         <v>0</v>
       </c>
       <c r="E49" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F49">
         <v>0</v>
       </c>
       <c r="H49">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I49" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I49" t="e">
-        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q49" t="s">
@@ -16619,7 +16624,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="str">
-        <f>VLOOKUP(A50,Q50:V1985,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C50">
@@ -16629,18 +16634,18 @@
         <v>0</v>
       </c>
       <c r="E50" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F50">
         <v>0</v>
       </c>
       <c r="H50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I50" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I50" t="e">
-        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q50" t="s">
@@ -16667,7 +16672,7 @@
         <v>52</v>
       </c>
       <c r="B51" t="str">
-        <f>VLOOKUP(A51,Q51:V1986,6)</f>
+        <f t="shared" si="4"/>
         <v>Residential</v>
       </c>
       <c r="C51">
@@ -16677,18 +16682,18 @@
         <v>0</v>
       </c>
       <c r="E51" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F51">
         <v>0</v>
       </c>
       <c r="H51">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I51" t="e">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I51" t="e">
-        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q51" t="s">

</xml_diff>